<commit_message>
Completed Config, Orchestrator Credentail, System1_Login
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uipath-my.sharepoint.com/personal/alexandra_veizu_uipath_com/Documents/Documents/Projects/REFrameworkNET5/StudioTemplates/REFramework/contentFiles/any/any/pt2/VisualBasic/Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Python\Documents\UiPath\Calculate_Client_Security_Hash_2023_Study\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{00D541BD-CB78-4D75-8532-9AD73E8C785E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F8C54E24-BA5C-4BF9-8DAB-2778512EC11B}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{271BDFDF-E192-45EB-8D7D-24E1BE063609}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="53">
   <si>
     <t>Name</t>
   </si>
@@ -85,9 +85,6 @@
   </si>
   <si>
     <t>logF_BusinessProcessName</t>
-  </si>
-  <si>
-    <t>Framework</t>
   </si>
   <si>
     <t>Orchestrator queue Name. The value must match with the queue name defined on Orchestrator.</t>
@@ -160,6 +157,33 @@
   </si>
   <si>
     <t>ProcessABCQueue</t>
+  </si>
+  <si>
+    <t>System1_URL</t>
+  </si>
+  <si>
+    <t>System1_Credential</t>
+  </si>
+  <si>
+    <t>SHA1_URL</t>
+  </si>
+  <si>
+    <t>CCSH-23</t>
+  </si>
+  <si>
+    <t>https://acme-test.uipath.com/</t>
+  </si>
+  <si>
+    <t>http://www.sha1-online.com/</t>
+  </si>
+  <si>
+    <t>SYSTEM1_CREDENTIAL</t>
+  </si>
+  <si>
+    <t>OrchestratorFolderPath</t>
+  </si>
+  <si>
+    <t>Shared</t>
   </si>
 </sst>
 </file>
@@ -211,16 +235,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+  <cellXfs count="6">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -535,18 +560,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z998"/>
+  <dimension ref="A1:Z997"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="43.5546875" customWidth="1"/>
+    <col min="1" max="1" width="43.5703125" customWidth="1"/>
     <col min="2" max="2" width="43" customWidth="1"/>
-    <col min="3" max="3" width="81.44140625" customWidth="1"/>
-    <col min="4" max="26" width="8.6640625" customWidth="1"/>
+    <col min="3" max="3" width="81.42578125" customWidth="1"/>
+    <col min="4" max="26" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -585,39 +610,67 @@
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1">
       <c r="A2" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="43.2">
+    <row r="3" spans="1:26" ht="45">
       <c r="A3" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B3" s="2"/>
       <c r="C3" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
-    <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="5" spans="1:26" ht="28.8">
+    <row r="4" spans="1:26" ht="30">
+      <c r="A4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:26" ht="14.25" customHeight="1">
       <c r="A5" t="s">
-        <v>20</v>
-      </c>
-      <c r="B5" t="s">
-        <v>21</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>23</v>
+        <v>44</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>48</v>
       </c>
     </row>
-    <row r="6" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="7" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="8" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="6" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A6" t="s">
+        <v>45</v>
+      </c>
+      <c r="B6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="7" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A7" t="s">
+        <v>46</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="8" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A8" t="s">
+        <v>51</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>52</v>
+      </c>
+    </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="10" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
@@ -1607,7 +1660,6 @@
     <row r="995" ht="14.25" customHeight="1"/>
     <row r="996" ht="14.25" customHeight="1"/>
     <row r="997" ht="14.25" customHeight="1"/>
-    <row r="998" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1620,15 +1672,15 @@
   <dimension ref="A1:Z988"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="41" customWidth="1"/>
     <col min="2" max="2" width="51" customWidth="1"/>
-    <col min="3" max="3" width="75.44140625" customWidth="1"/>
-    <col min="4" max="26" width="8.6640625" customWidth="1"/>
+    <col min="3" max="3" width="75.42578125" customWidth="1"/>
+    <col min="4" max="26" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -1665,26 +1717,26 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" ht="28.8">
+    <row r="2" spans="1:26" ht="30">
       <c r="A2" t="s">
         <v>5</v>
       </c>
       <c r="B2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="43.2">
+    <row r="3" spans="1:26" ht="45">
       <c r="A3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B3">
         <v>0</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
@@ -1708,7 +1760,7 @@
         <v>10</v>
       </c>
       <c r="C7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
@@ -1730,7 +1782,7 @@
         <v>15</v>
       </c>
       <c r="C9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1">
@@ -1741,7 +1793,7 @@
         <v>17</v>
       </c>
       <c r="C10" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1">
@@ -1752,53 +1804,53 @@
         <v>19</v>
       </c>
       <c r="C11" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1">
       <c r="A12" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B12" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C12" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="14" spans="1:26" ht="14.25" customHeight="1">
       <c r="A14" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B14">
         <v>2</v>
       </c>
       <c r="C14" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1">
       <c r="A15" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B15">
         <v>2</v>
       </c>
       <c r="C15" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="17" spans="1:3" ht="28.8">
+    <row r="17" spans="1:3" ht="45">
       <c r="A17" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B17" t="b">
         <v>0</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="14.25" customHeight="1"/>
@@ -2782,14 +2834,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="31.88671875" customWidth="1"/>
-    <col min="2" max="2" width="30.109375" customWidth="1"/>
-    <col min="3" max="3" width="60.33203125" customWidth="1"/>
-    <col min="4" max="26" width="65.44140625" customWidth="1"/>
+    <col min="1" max="1" width="31.85546875" customWidth="1"/>
+    <col min="2" max="2" width="30.140625" customWidth="1"/>
+    <col min="3" max="3" width="60.28515625" customWidth="1"/>
+    <col min="4" max="26" width="65.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -2800,7 +2854,7 @@
         <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>4</v>

</xml_diff>